<commit_message>
modified:   1_satge_volume.xlsx 	modified:   1_stage.xlsx 	modified:   2_stage.xlsx 	modified:   2_stage_volume.xlsx 	modified:   cost_price 1 stage.xlsx 	modified:   cost_price.xlsx 	modified:   defectura.xlsx 	modified:   expenses.xlsx 	modified:   finish_goods_stocks.xlsx 	modified:   raw_mat_bad_stock.xlsx 	modified:   report.pbix 	modified:   sales_extend.xlsx 	modified:   stock_analysis.ipynb 	modified:   stock_analysis.xlsx
</commit_message>
<xml_diff>
--- a/1_stage.xlsx
+++ b/1_stage.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1950" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1962" uniqueCount="147">
   <si>
     <t>Месяц</t>
   </si>
@@ -461,6 +461,9 @@
   <si>
     <t>01.10.2022</t>
   </si>
+  <si>
+    <t>01.11.2022</t>
+  </si>
 </sst>
 </file>
 
@@ -881,10 +884,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:H972"/>
+  <dimension ref="A1:H978"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A935" workbookViewId="0">
-      <selection activeCell="A966" sqref="A966:H972"/>
+      <selection activeCell="A973" sqref="A973:H978"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="11.45" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24228,6 +24231,150 @@
         <v>404.34</v>
       </c>
     </row>
+    <row r="973" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A973" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B973" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C973" s="8">
+        <v>1678</v>
+      </c>
+      <c r="D973" s="6"/>
+      <c r="E973" s="7">
+        <v>10.67</v>
+      </c>
+      <c r="F973" s="7">
+        <v>279.67</v>
+      </c>
+      <c r="G973" s="7">
+        <v>6</v>
+      </c>
+      <c r="H973" s="7">
+        <v>9.83</v>
+      </c>
+    </row>
+    <row r="974" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A974" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B974" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C974" s="8">
+        <v>10444.4</v>
+      </c>
+      <c r="D974" s="6"/>
+      <c r="E974" s="7">
+        <v>79.819999999999993</v>
+      </c>
+      <c r="F974" s="7">
+        <v>356.1</v>
+      </c>
+      <c r="G974" s="7">
+        <v>29.33</v>
+      </c>
+      <c r="H974" s="7">
+        <v>52.34</v>
+      </c>
+    </row>
+    <row r="975" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A975" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B975" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C975" s="5">
+        <v>413.2</v>
+      </c>
+      <c r="D975" s="6"/>
+      <c r="E975" s="7">
+        <v>17</v>
+      </c>
+      <c r="F975" s="7">
+        <v>28.5</v>
+      </c>
+      <c r="G975" s="7">
+        <v>14.5</v>
+      </c>
+      <c r="H975" s="7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="976" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A976" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B976" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C976" s="8">
+        <v>6455</v>
+      </c>
+      <c r="D976" s="6"/>
+      <c r="E976" s="7">
+        <v>99.49</v>
+      </c>
+      <c r="F976" s="7">
+        <v>241.22</v>
+      </c>
+      <c r="G976" s="7">
+        <v>26.76</v>
+      </c>
+      <c r="H976" s="7">
+        <v>52.76</v>
+      </c>
+    </row>
+    <row r="977" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A977" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B977" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C977" s="8">
+        <v>8003</v>
+      </c>
+      <c r="D977" s="6"/>
+      <c r="E977" s="7">
+        <v>117.51</v>
+      </c>
+      <c r="F977" s="7">
+        <v>245.64</v>
+      </c>
+      <c r="G977" s="7">
+        <v>32.58</v>
+      </c>
+      <c r="H977" s="7">
+        <v>68.25</v>
+      </c>
+    </row>
+    <row r="978" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A978" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B978" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C978" s="8">
+        <v>3028.5</v>
+      </c>
+      <c r="D978" s="6"/>
+      <c r="E978" s="7">
+        <v>63.5</v>
+      </c>
+      <c r="F978" s="7">
+        <v>169</v>
+      </c>
+      <c r="G978" s="7">
+        <v>17.920000000000002</v>
+      </c>
+      <c r="H978" s="7">
+        <v>39.159999999999997</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H901">
     <sortState ref="A2:H914">

</xml_diff>

<commit_message>
deleted:    .idea/.gitignore 	deleted:    .idea/KPI PBI.iml 	deleted:    .idea/deployment.xml 	deleted:    .idea/inspectionProfiles/Project_Default.xml 	deleted:    .idea/inspectionProfiles/profiles_settings.xml 	deleted:    .idea/misc.xml 	deleted:    .idea/modules.xml 	deleted:    .idea/other.xml 	modified:   1_satge_volume.xlsx 	modified:   1_stage.xlsx 	modified:   2_stage.xlsx 	modified:   2_stage_volume.xlsx 	modified:   defectura.xlsx 	modified:   expenses.xlsx 	modified:   finish_goods_stocks.xlsx 	modified:   raw_mat_bad_stock.xlsx 	modified:   report.pbix 	modified:   sales_extend.xlsx 	modified:   stock_analysis.ipynb 	modified:   stock_analysis.xlsx 	deleted:    test.py 	modified:   time_series_10_22.pkl
</commit_message>
<xml_diff>
--- a/1_stage.xlsx
+++ b/1_stage.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1962" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1964" uniqueCount="147">
   <si>
     <t>Месяц</t>
   </si>
@@ -884,10 +884,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:H978"/>
+  <dimension ref="A1:H979"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A935" workbookViewId="0">
-      <selection activeCell="A973" sqref="A973:H978"/>
+      <selection activeCell="A973" sqref="A973:H979"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="11.45" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24260,23 +24260,23 @@
         <v>146</v>
       </c>
       <c r="B974" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C974" s="8">
-        <v>10444.4</v>
+        <v>9375</v>
       </c>
       <c r="D974" s="6"/>
       <c r="E974" s="7">
-        <v>79.819999999999993</v>
+        <v>45.67</v>
       </c>
       <c r="F974" s="7">
-        <v>356.1</v>
+        <v>400.47</v>
       </c>
       <c r="G974" s="7">
-        <v>29.33</v>
+        <v>23.41</v>
       </c>
       <c r="H974" s="7">
-        <v>52.34</v>
+        <v>28.33</v>
       </c>
     </row>
     <row r="975" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24284,23 +24284,23 @@
         <v>146</v>
       </c>
       <c r="B975" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C975" s="5">
-        <v>413.2</v>
+        <v>10</v>
+      </c>
+      <c r="C975" s="8">
+        <v>16997.900000000001</v>
       </c>
       <c r="D975" s="6"/>
       <c r="E975" s="7">
-        <v>17</v>
+        <v>120.82</v>
       </c>
       <c r="F975" s="7">
-        <v>28.5</v>
+        <v>341.12</v>
       </c>
       <c r="G975" s="7">
-        <v>14.5</v>
+        <v>49.83</v>
       </c>
       <c r="H975" s="7">
-        <v>18</v>
+        <v>84.25</v>
       </c>
     </row>
     <row r="976" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24308,23 +24308,23 @@
         <v>146</v>
       </c>
       <c r="B976" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C976" s="8">
-        <v>6455</v>
+        <v>11</v>
+      </c>
+      <c r="C976" s="5">
+        <v>828.2</v>
       </c>
       <c r="D976" s="6"/>
       <c r="E976" s="7">
-        <v>99.49</v>
+        <v>36.83</v>
       </c>
       <c r="F976" s="7">
-        <v>241.22</v>
+        <v>26.72</v>
       </c>
       <c r="G976" s="7">
-        <v>26.76</v>
+        <v>31</v>
       </c>
       <c r="H976" s="7">
-        <v>52.76</v>
+        <v>39.33</v>
       </c>
     </row>
     <row r="977" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24332,23 +24332,23 @@
         <v>146</v>
       </c>
       <c r="B977" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C977" s="8">
-        <v>8003</v>
+        <v>18224.099999999999</v>
       </c>
       <c r="D977" s="6"/>
       <c r="E977" s="7">
-        <v>117.51</v>
+        <v>224.5</v>
       </c>
       <c r="F977" s="7">
-        <v>245.64</v>
+        <v>262.48</v>
       </c>
       <c r="G977" s="7">
-        <v>32.58</v>
+        <v>69.430000000000007</v>
       </c>
       <c r="H977" s="7">
-        <v>68.25</v>
+        <v>119.58</v>
       </c>
     </row>
     <row r="978" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24356,23 +24356,47 @@
         <v>146</v>
       </c>
       <c r="B978" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C978" s="8">
-        <v>3028.5</v>
+        <v>9865</v>
       </c>
       <c r="D978" s="6"/>
       <c r="E978" s="7">
-        <v>63.5</v>
+        <v>137.18</v>
       </c>
       <c r="F978" s="7">
-        <v>169</v>
+        <v>246.13</v>
       </c>
       <c r="G978" s="7">
-        <v>17.920000000000002</v>
+        <v>40.08</v>
       </c>
       <c r="H978" s="7">
-        <v>39.159999999999997</v>
+        <v>78.58</v>
+      </c>
+    </row>
+    <row r="979" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A979" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B979" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C979" s="8">
+        <v>3885.5</v>
+      </c>
+      <c r="D979" s="6"/>
+      <c r="E979" s="7">
+        <v>91.33</v>
+      </c>
+      <c r="F979" s="7">
+        <v>156.41999999999999</v>
+      </c>
+      <c r="G979" s="7">
+        <v>24.84</v>
+      </c>
+      <c r="H979" s="7">
+        <v>55.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   1_satge_volume.xlsx 	modified:   1_stage.xlsx 	modified:   2_stage.xlsx 	modified:   2_stage_volume.xlsx 	modified:   expenses.xlsx 	modified:   finish_goods_stocks.xlsx 	modified:   raw_mat_bad_stock.xlsx 	modified:   report.pbix 	modified:   sales_extend.xlsx 	modified:   stock_analysis.ipynb 	modified:   stock_analysis.xlsx
</commit_message>
<xml_diff>
--- a/1_stage.xlsx
+++ b/1_stage.xlsx
@@ -24263,20 +24263,20 @@
         <v>9</v>
       </c>
       <c r="C974" s="8">
-        <v>9375</v>
+        <v>20847.2</v>
       </c>
       <c r="D974" s="6"/>
       <c r="E974" s="7">
-        <v>45.67</v>
+        <v>106.42</v>
       </c>
       <c r="F974" s="7">
-        <v>400.47</v>
+        <v>355.94</v>
       </c>
       <c r="G974" s="7">
-        <v>23.41</v>
+        <v>58.57</v>
       </c>
       <c r="H974" s="7">
-        <v>28.33</v>
+        <v>81.83</v>
       </c>
     </row>
     <row r="975" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24287,20 +24287,20 @@
         <v>10</v>
       </c>
       <c r="C975" s="8">
-        <v>16997.900000000001</v>
+        <v>23966</v>
       </c>
       <c r="D975" s="6"/>
       <c r="E975" s="7">
-        <v>120.82</v>
+        <v>174.31</v>
       </c>
       <c r="F975" s="7">
-        <v>341.12</v>
+        <v>338.36</v>
       </c>
       <c r="G975" s="7">
-        <v>49.83</v>
+        <v>70.83</v>
       </c>
       <c r="H975" s="7">
-        <v>84.25</v>
+        <v>120.17</v>
       </c>
     </row>
     <row r="976" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24310,21 +24310,21 @@
       <c r="B976" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C976" s="5">
-        <v>828.2</v>
+      <c r="C976" s="8">
+        <v>1232</v>
       </c>
       <c r="D976" s="6"/>
       <c r="E976" s="7">
-        <v>36.83</v>
+        <v>55.5</v>
       </c>
       <c r="F976" s="7">
-        <v>26.72</v>
+        <v>26.49</v>
       </c>
       <c r="G976" s="7">
-        <v>31</v>
+        <v>46.5</v>
       </c>
       <c r="H976" s="7">
-        <v>39.33</v>
+        <v>59</v>
       </c>
     </row>
     <row r="977" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24335,20 +24335,20 @@
         <v>12</v>
       </c>
       <c r="C977" s="8">
-        <v>18224.099999999999</v>
+        <v>30082.3</v>
       </c>
       <c r="D977" s="6"/>
       <c r="E977" s="7">
-        <v>224.5</v>
+        <v>356.34</v>
       </c>
       <c r="F977" s="7">
-        <v>262.48</v>
+        <v>263.05</v>
       </c>
       <c r="G977" s="7">
-        <v>69.430000000000007</v>
+        <v>114.36</v>
       </c>
       <c r="H977" s="7">
-        <v>119.58</v>
+        <v>190.65</v>
       </c>
     </row>
     <row r="978" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24359,20 +24359,20 @@
         <v>13</v>
       </c>
       <c r="C978" s="8">
-        <v>9865</v>
+        <v>13760.6</v>
       </c>
       <c r="D978" s="6"/>
       <c r="E978" s="7">
-        <v>137.18</v>
+        <v>200.52</v>
       </c>
       <c r="F978" s="7">
-        <v>246.13</v>
+        <v>240.36</v>
       </c>
       <c r="G978" s="7">
-        <v>40.08</v>
+        <v>57.25</v>
       </c>
       <c r="H978" s="7">
-        <v>78.58</v>
+        <v>114.41</v>
       </c>
     </row>
     <row r="979" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24383,20 +24383,20 @@
         <v>14</v>
       </c>
       <c r="C979" s="8">
-        <v>3885.5</v>
+        <v>11018.5</v>
       </c>
       <c r="D979" s="6"/>
       <c r="E979" s="7">
-        <v>91.33</v>
+        <v>198.74</v>
       </c>
       <c r="F979" s="7">
-        <v>156.41999999999999</v>
+        <v>183.37</v>
       </c>
       <c r="G979" s="7">
-        <v>24.84</v>
+        <v>60.09</v>
       </c>
       <c r="H979" s="7">
-        <v>55.83</v>
+        <v>122.26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   1_satge_volume.xlsx 	modified:   1_stage.xlsx 	modified:   2_stage.xlsx 	modified:   2_stage_volume.xlsx 	modified:   defectura.xlsx 	modified:   expenses.xlsx 	modified:   finish_goods_stocks.xlsx 	modified:   raw_mat_bad_stock.xlsx 	modified:   report.pbix 	modified:   sales_extend.xlsx 	modified:   stock_analysis.xlsx 	modified:   stock_analysis_final.xlsx 	modified:   streamlit_app.py
</commit_message>
<xml_diff>
--- a/1_stage.xlsx
+++ b/1_stage.xlsx
@@ -24263,20 +24263,20 @@
         <v>9</v>
       </c>
       <c r="C974" s="8">
-        <v>20847.2</v>
+        <v>30512.2</v>
       </c>
       <c r="D974" s="6"/>
       <c r="E974" s="7">
-        <v>106.42</v>
+        <v>197.41</v>
       </c>
       <c r="F974" s="7">
-        <v>355.94</v>
+        <v>337.86</v>
       </c>
       <c r="G974" s="7">
-        <v>58.57</v>
+        <v>90.31</v>
       </c>
       <c r="H974" s="7">
-        <v>81.83</v>
+        <v>129.84</v>
       </c>
     </row>
     <row r="975" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24287,20 +24287,20 @@
         <v>10</v>
       </c>
       <c r="C975" s="8">
-        <v>23966</v>
+        <v>27134.6</v>
       </c>
       <c r="D975" s="6"/>
       <c r="E975" s="7">
-        <v>174.31</v>
+        <v>206.15</v>
       </c>
       <c r="F975" s="7">
-        <v>338.36</v>
+        <v>338.17</v>
       </c>
       <c r="G975" s="7">
-        <v>70.83</v>
+        <v>80.239999999999995</v>
       </c>
       <c r="H975" s="7">
-        <v>120.17</v>
+        <v>139.41999999999999</v>
       </c>
     </row>
     <row r="976" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24311,20 +24311,20 @@
         <v>11</v>
       </c>
       <c r="C976" s="8">
-        <v>1232</v>
+        <v>1961</v>
       </c>
       <c r="D976" s="6"/>
       <c r="E976" s="7">
-        <v>55.5</v>
+        <v>88</v>
       </c>
       <c r="F976" s="7">
-        <v>26.49</v>
+        <v>26.86</v>
       </c>
       <c r="G976" s="7">
-        <v>46.5</v>
+        <v>73</v>
       </c>
       <c r="H976" s="7">
-        <v>59</v>
+        <v>93.5</v>
       </c>
     </row>
     <row r="977" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24335,20 +24335,20 @@
         <v>12</v>
       </c>
       <c r="C977" s="8">
-        <v>30082.3</v>
+        <v>35065.300000000003</v>
       </c>
       <c r="D977" s="6"/>
       <c r="E977" s="7">
-        <v>356.34</v>
+        <v>421.75</v>
       </c>
       <c r="F977" s="7">
-        <v>263.05</v>
+        <v>250.39</v>
       </c>
       <c r="G977" s="7">
-        <v>114.36</v>
+        <v>140.04</v>
       </c>
       <c r="H977" s="7">
-        <v>190.65</v>
+        <v>233.82</v>
       </c>
     </row>
     <row r="978" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24359,20 +24359,20 @@
         <v>13</v>
       </c>
       <c r="C978" s="8">
-        <v>13760.6</v>
+        <v>19888.3</v>
       </c>
       <c r="D978" s="6"/>
       <c r="E978" s="7">
-        <v>200.52</v>
+        <v>299.52</v>
       </c>
       <c r="F978" s="7">
-        <v>240.36</v>
+        <v>202.88</v>
       </c>
       <c r="G978" s="7">
-        <v>57.25</v>
+        <v>98.03</v>
       </c>
       <c r="H978" s="7">
-        <v>114.41</v>
+        <v>182.57</v>
       </c>
     </row>
     <row r="979" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24383,20 +24383,20 @@
         <v>14</v>
       </c>
       <c r="C979" s="8">
-        <v>11018.5</v>
+        <v>16664</v>
       </c>
       <c r="D979" s="6"/>
       <c r="E979" s="7">
-        <v>198.74</v>
+        <v>295.58</v>
       </c>
       <c r="F979" s="7">
-        <v>183.37</v>
+        <v>190.97</v>
       </c>
       <c r="G979" s="7">
-        <v>60.09</v>
+        <v>87.26</v>
       </c>
       <c r="H979" s="7">
-        <v>122.26</v>
+        <v>173.17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   1_satge_volume.xlsx 	modified:   1_stage.xlsx 	modified:   2_stage.xlsx 	modified:   2_stage_volume.xlsx 	modified:   defectura.xlsx 	modified:   expenses.xlsx 	modified:   finish_goods_stocks.xlsx 	modified:   raw_mat_bad_stock.xlsx 	modified:   report.pbix 	modified:   sales_extend.xlsx 	modified:   stock_analysis.ipynb 	modified:   stock_analysis.xlsx 	modified:   stock_analysis_final.xlsx
</commit_message>
<xml_diff>
--- a/1_stage.xlsx
+++ b/1_stage.xlsx
@@ -24263,20 +24263,20 @@
         <v>9</v>
       </c>
       <c r="C974" s="8">
-        <v>30512.2</v>
+        <v>32952.199999999997</v>
       </c>
       <c r="D974" s="6"/>
       <c r="E974" s="7">
-        <v>197.41</v>
+        <v>214.07</v>
       </c>
       <c r="F974" s="7">
-        <v>337.86</v>
+        <v>343.65</v>
       </c>
       <c r="G974" s="7">
-        <v>90.31</v>
+        <v>95.89</v>
       </c>
       <c r="H974" s="7">
-        <v>129.84</v>
+        <v>138.68</v>
       </c>
     </row>
     <row r="975" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24287,20 +24287,20 @@
         <v>10</v>
       </c>
       <c r="C975" s="8">
-        <v>27134.6</v>
+        <v>31876.400000000001</v>
       </c>
       <c r="D975" s="6"/>
       <c r="E975" s="7">
-        <v>206.15</v>
+        <v>232.81</v>
       </c>
       <c r="F975" s="7">
-        <v>338.17</v>
+        <v>330.63</v>
       </c>
       <c r="G975" s="7">
-        <v>80.239999999999995</v>
+        <v>96.41</v>
       </c>
       <c r="H975" s="7">
-        <v>139.41999999999999</v>
+        <v>168.08</v>
       </c>
     </row>
     <row r="976" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24335,20 +24335,20 @@
         <v>12</v>
       </c>
       <c r="C977" s="8">
-        <v>35065.300000000003</v>
+        <v>39014</v>
       </c>
       <c r="D977" s="6"/>
       <c r="E977" s="7">
-        <v>421.75</v>
+        <v>475.42</v>
       </c>
       <c r="F977" s="7">
-        <v>250.39</v>
+        <v>252.99</v>
       </c>
       <c r="G977" s="7">
-        <v>140.04</v>
+        <v>154.21</v>
       </c>
       <c r="H977" s="7">
-        <v>233.82</v>
+        <v>262.14999999999998</v>
       </c>
     </row>
     <row r="978" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24359,20 +24359,20 @@
         <v>13</v>
       </c>
       <c r="C978" s="8">
-        <v>19888.3</v>
+        <v>23069</v>
       </c>
       <c r="D978" s="6"/>
       <c r="E978" s="7">
-        <v>299.52</v>
+        <v>350.86</v>
       </c>
       <c r="F978" s="7">
-        <v>202.88</v>
+        <v>206.08</v>
       </c>
       <c r="G978" s="7">
-        <v>98.03</v>
+        <v>111.94</v>
       </c>
       <c r="H978" s="7">
-        <v>182.57</v>
+        <v>209.73</v>
       </c>
     </row>
     <row r="979" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24383,20 +24383,20 @@
         <v>14</v>
       </c>
       <c r="C979" s="8">
-        <v>16664</v>
+        <v>20006.8</v>
       </c>
       <c r="D979" s="6"/>
       <c r="E979" s="7">
-        <v>295.58</v>
+        <v>355.25</v>
       </c>
       <c r="F979" s="7">
-        <v>190.97</v>
+        <v>182.84</v>
       </c>
       <c r="G979" s="7">
-        <v>87.26</v>
+        <v>109.42</v>
       </c>
       <c r="H979" s="7">
-        <v>173.17</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   1_satge_volume.xlsx 	modified:   1_stage.xlsx 	modified:   2_stage.xlsx 	modified:   2_stage_volume.xlsx 	modified:   defectura.xlsx 	modified:   expenses.xlsx 	modified:   finish_goods_stocks.xlsx 	modified:   report.pbix 	modified:   sales_extend.xlsx 	modified:   stock_analysis.xlsx 	modified:   stock_analysis_final.xlsx
</commit_message>
<xml_diff>
--- a/1_stage.xlsx
+++ b/1_stage.xlsx
@@ -24263,20 +24263,20 @@
         <v>9</v>
       </c>
       <c r="C974" s="8">
-        <v>52885.7</v>
+        <v>60585.7</v>
       </c>
       <c r="D974" s="6"/>
       <c r="E974" s="7">
-        <v>335.24</v>
+        <v>360.24</v>
       </c>
       <c r="F974" s="7">
-        <v>317.23</v>
+        <v>321.79000000000002</v>
       </c>
       <c r="G974" s="7">
-        <v>166.71</v>
+        <v>188.28</v>
       </c>
       <c r="H974" s="7">
-        <v>231.18</v>
+        <v>257.68</v>
       </c>
     </row>
     <row r="975" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24287,20 +24287,20 @@
         <v>10</v>
       </c>
       <c r="C975" s="8">
-        <v>40310</v>
+        <v>44079.1</v>
       </c>
       <c r="D975" s="6"/>
       <c r="E975" s="7">
-        <v>301.97000000000003</v>
+        <v>327.3</v>
       </c>
       <c r="F975" s="7">
-        <v>299.68</v>
+        <v>303.60000000000002</v>
       </c>
       <c r="G975" s="7">
-        <v>134.51</v>
+        <v>145.19</v>
       </c>
       <c r="H975" s="7">
-        <v>233.24</v>
+        <v>251.73</v>
       </c>
     </row>
     <row r="976" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24359,20 +24359,20 @@
         <v>13</v>
       </c>
       <c r="C978" s="8">
-        <v>33925.599999999999</v>
+        <v>34684.1</v>
       </c>
       <c r="D978" s="6"/>
       <c r="E978" s="7">
-        <v>501.86</v>
+        <v>517.20000000000005</v>
       </c>
       <c r="F978" s="7">
-        <v>206.74</v>
+        <v>204.41</v>
       </c>
       <c r="G978" s="7">
-        <v>164.1</v>
+        <v>169.68</v>
       </c>
       <c r="H978" s="7">
-        <v>298.23</v>
+        <v>307.73</v>
       </c>
     </row>
     <row r="979" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24383,20 +24383,20 @@
         <v>14</v>
       </c>
       <c r="C979" s="8">
-        <v>24176.799999999999</v>
+        <v>30427.8</v>
       </c>
       <c r="D979" s="6"/>
       <c r="E979" s="7">
-        <v>438.25</v>
+        <v>493.92</v>
       </c>
       <c r="F979" s="7">
-        <v>187.78</v>
+        <v>201.39</v>
       </c>
       <c r="G979" s="7">
-        <v>128.75</v>
+        <v>151.09</v>
       </c>
       <c r="H979" s="7">
-        <v>249</v>
+        <v>278.33</v>
       </c>
     </row>
     <row r="980" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24407,20 +24407,20 @@
         <v>15</v>
       </c>
       <c r="C980" s="8">
-        <v>3996.3</v>
+        <v>6933.6</v>
       </c>
       <c r="D980" s="6"/>
       <c r="E980" s="7">
-        <v>48</v>
+        <v>83.17</v>
       </c>
       <c r="F980" s="7">
-        <v>244.72</v>
+        <v>220.11</v>
       </c>
       <c r="G980" s="7">
-        <v>16.329999999999998</v>
+        <v>31.5</v>
       </c>
       <c r="H980" s="7">
-        <v>25.5</v>
+        <v>45.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   1_satge_volume.xlsx 	modified:   1_stage.xlsx 	modified:   2_stage.xlsx 	modified:   2_stage_volume.xlsx 	modified:   defectura.xlsx 	modified:   expenses.xlsx 	modified:   finish_goods_stocks.xlsx 	modified:   raw_mat_bad_stock.xlsx 	modified:   report.pbix 	modified:   sales_extend.xlsx 	modified:   stock_analysis.ipynb 	modified:   stock_analysis.xlsx 	modified:   stock_analysis_final.xlsx 	new file:   time_series_11_22.pkl
</commit_message>
<xml_diff>
--- a/1_stage.xlsx
+++ b/1_stage.xlsx
@@ -24263,20 +24263,20 @@
         <v>9</v>
       </c>
       <c r="C974" s="8">
-        <v>60585.7</v>
+        <v>68529.7</v>
       </c>
       <c r="D974" s="6"/>
       <c r="E974" s="7">
-        <v>360.24</v>
+        <v>386.41</v>
       </c>
       <c r="F974" s="7">
-        <v>321.79000000000002</v>
+        <v>325.37</v>
       </c>
       <c r="G974" s="7">
-        <v>188.28</v>
+        <v>210.62</v>
       </c>
       <c r="H974" s="7">
-        <v>257.68</v>
+        <v>285.35000000000002</v>
       </c>
     </row>
     <row r="975" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24287,20 +24287,20 @@
         <v>10</v>
       </c>
       <c r="C975" s="8">
-        <v>44079.1</v>
+        <v>48214.6</v>
       </c>
       <c r="D975" s="6"/>
       <c r="E975" s="7">
-        <v>327.3</v>
+        <v>350.31</v>
       </c>
       <c r="F975" s="7">
-        <v>303.60000000000002</v>
+        <v>300.98</v>
       </c>
       <c r="G975" s="7">
-        <v>145.19</v>
+        <v>160.19</v>
       </c>
       <c r="H975" s="7">
-        <v>251.73</v>
+        <v>276.24</v>
       </c>
     </row>
     <row r="976" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24311,20 +24311,20 @@
         <v>11</v>
       </c>
       <c r="C976" s="8">
-        <v>2424.4</v>
+        <v>3414.1</v>
       </c>
       <c r="D976" s="6"/>
       <c r="E976" s="7">
-        <v>110.5</v>
+        <v>140.5</v>
       </c>
       <c r="F976" s="7">
-        <v>26.57</v>
+        <v>29.12</v>
       </c>
       <c r="G976" s="7">
-        <v>91.25</v>
+        <v>117.25</v>
       </c>
       <c r="H976" s="7">
-        <v>118</v>
+        <v>150</v>
       </c>
     </row>
     <row r="977" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24359,20 +24359,20 @@
         <v>13</v>
       </c>
       <c r="C978" s="8">
-        <v>34684.1</v>
+        <v>39637.1</v>
       </c>
       <c r="D978" s="6"/>
       <c r="E978" s="7">
-        <v>517.20000000000005</v>
+        <v>592.70000000000005</v>
       </c>
       <c r="F978" s="7">
-        <v>204.41</v>
+        <v>205.73</v>
       </c>
       <c r="G978" s="7">
-        <v>169.68</v>
+        <v>192.67</v>
       </c>
       <c r="H978" s="7">
-        <v>307.73</v>
+        <v>351.23</v>
       </c>
     </row>
     <row r="979" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24383,20 +24383,20 @@
         <v>14</v>
       </c>
       <c r="C979" s="8">
-        <v>30427.8</v>
+        <v>36792.800000000003</v>
       </c>
       <c r="D979" s="6"/>
       <c r="E979" s="7">
-        <v>493.92</v>
+        <v>549.91999999999996</v>
       </c>
       <c r="F979" s="7">
-        <v>201.39</v>
+        <v>212.66</v>
       </c>
       <c r="G979" s="7">
-        <v>151.09</v>
+        <v>173.01</v>
       </c>
       <c r="H979" s="7">
-        <v>278.33</v>
+        <v>310</v>
       </c>
     </row>
     <row r="980" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
modified:   1_satge_volume.xlsx 	modified:   1_stage.xlsx 	modified:   2_stage.xlsx 	modified:   2_stage_volume.xlsx 	modified:   cost_price 1 stage.xlsx 	modified:   defectura.xlsx 	modified:   expenses.xlsx 	modified:   finish_goods_stocks.xlsx 	modified:   raw_mat_bad_stock.xlsx 	modified:   report.pbix 	modified:   sales_extend.xlsx 	modified:   stock_analysis.ipynb 	modified:   stock_analysis.xlsx 	modified:   stock_analysis_final.xlsx
</commit_message>
<xml_diff>
--- a/1_stage.xlsx
+++ b/1_stage.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1966" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1976" uniqueCount="148">
   <si>
     <t>Месяц</t>
   </si>
@@ -464,6 +464,9 @@
   <si>
     <t>01.11.2022</t>
   </si>
+  <si>
+    <t>01.12.2022</t>
+  </si>
 </sst>
 </file>
 
@@ -884,10 +887,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:H980"/>
+  <dimension ref="A1:H985"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A935" workbookViewId="0">
-      <selection activeCell="A973" sqref="A973:H980"/>
+    <sheetView tabSelected="1" topLeftCell="A971" workbookViewId="0">
+      <selection activeCell="A981" sqref="A981:H985"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="11.45" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24423,6 +24426,126 @@
         <v>45.67</v>
       </c>
     </row>
+    <row r="981" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A981" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B981" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C981" s="8">
+        <v>15659.1</v>
+      </c>
+      <c r="D981" s="6"/>
+      <c r="E981" s="7">
+        <v>101.74</v>
+      </c>
+      <c r="F981" s="7">
+        <v>405.15</v>
+      </c>
+      <c r="G981" s="7">
+        <v>38.65</v>
+      </c>
+      <c r="H981" s="7">
+        <v>55.26</v>
+      </c>
+    </row>
+    <row r="982" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A982" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B982" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C982" s="8">
+        <v>8229.2999999999993</v>
+      </c>
+      <c r="D982" s="6"/>
+      <c r="E982" s="7">
+        <v>60.59</v>
+      </c>
+      <c r="F982" s="7">
+        <v>262</v>
+      </c>
+      <c r="G982" s="7">
+        <v>31.41</v>
+      </c>
+      <c r="H982" s="7">
+        <v>52.75</v>
+      </c>
+    </row>
+    <row r="983" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A983" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B983" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C983" s="5">
+        <v>235.5</v>
+      </c>
+      <c r="D983" s="6"/>
+      <c r="E983" s="7">
+        <v>11.17</v>
+      </c>
+      <c r="F983" s="7">
+        <v>26.4</v>
+      </c>
+      <c r="G983" s="7">
+        <v>8.92</v>
+      </c>
+      <c r="H983" s="7">
+        <v>11.67</v>
+      </c>
+    </row>
+    <row r="984" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A984" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B984" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C984" s="8">
+        <v>4246</v>
+      </c>
+      <c r="D984" s="6"/>
+      <c r="E984" s="7">
+        <v>68.59</v>
+      </c>
+      <c r="F984" s="7">
+        <v>213.26</v>
+      </c>
+      <c r="G984" s="7">
+        <v>19.91</v>
+      </c>
+      <c r="H984" s="7">
+        <v>34.08</v>
+      </c>
+    </row>
+    <row r="985" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A985" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B985" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C985" s="8">
+        <v>9214.7999999999993</v>
+      </c>
+      <c r="D985" s="6"/>
+      <c r="E985" s="7">
+        <v>136</v>
+      </c>
+      <c r="F985" s="7">
+        <v>242.43</v>
+      </c>
+      <c r="G985" s="7">
+        <v>38.01</v>
+      </c>
+      <c r="H985" s="7">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H901">
     <sortState ref="A2:H914">

</xml_diff>

<commit_message>
modified:   1_satge_volume.xlsx 	modified:   1_stage.xlsx 	modified:   2_stage.xlsx 	modified:   2_stage_volume.xlsx 	modified:   cost_price 1 stage.xlsx 	modified:   cost_price.xlsx 	modified:   defectura.xlsx 	modified:   expenses.xlsx 	modified:   finish_goods_stocks.xlsx 	modified:   raw_mat_bad_stock.xlsx 	modified:   report.pbix 	modified:   sales_extend.xlsx 	modified:   stock_analysis.ipynb 	modified:   stock_analysis.xlsx 	modified:   stock_analysis_final.xlsx
</commit_message>
<xml_diff>
--- a/1_stage.xlsx
+++ b/1_stage.xlsx
@@ -24434,20 +24434,20 @@
         <v>9</v>
       </c>
       <c r="C981" s="8">
-        <v>15659.1</v>
+        <v>25562.1</v>
       </c>
       <c r="D981" s="6"/>
       <c r="E981" s="7">
-        <v>101.74</v>
+        <v>151.41</v>
       </c>
       <c r="F981" s="7">
-        <v>405.15</v>
+        <v>379.77</v>
       </c>
       <c r="G981" s="7">
-        <v>38.65</v>
+        <v>67.31</v>
       </c>
       <c r="H981" s="7">
-        <v>55.26</v>
+        <v>90.09</v>
       </c>
     </row>
     <row r="982" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24458,20 +24458,20 @@
         <v>10</v>
       </c>
       <c r="C982" s="8">
-        <v>8229.2999999999993</v>
+        <v>13406.8</v>
       </c>
       <c r="D982" s="6"/>
       <c r="E982" s="7">
-        <v>60.59</v>
+        <v>111.84</v>
       </c>
       <c r="F982" s="7">
-        <v>262</v>
+        <v>275.07</v>
       </c>
       <c r="G982" s="7">
-        <v>31.41</v>
+        <v>48.74</v>
       </c>
       <c r="H982" s="7">
-        <v>52.75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="983" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24482,20 +24482,20 @@
         <v>11</v>
       </c>
       <c r="C983" s="5">
-        <v>235.5</v>
+        <v>385.5</v>
       </c>
       <c r="D983" s="6"/>
       <c r="E983" s="7">
-        <v>11.17</v>
+        <v>18.670000000000002</v>
       </c>
       <c r="F983" s="7">
-        <v>26.4</v>
+        <v>26.28</v>
       </c>
       <c r="G983" s="7">
-        <v>8.92</v>
+        <v>14.67</v>
       </c>
       <c r="H983" s="7">
-        <v>11.67</v>
+        <v>19.670000000000002</v>
       </c>
     </row>
     <row r="984" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24506,20 +24506,20 @@
         <v>13</v>
       </c>
       <c r="C984" s="8">
-        <v>4246</v>
+        <v>7544</v>
       </c>
       <c r="D984" s="6"/>
       <c r="E984" s="7">
-        <v>68.59</v>
+        <v>138.41999999999999</v>
       </c>
       <c r="F984" s="7">
-        <v>213.26</v>
+        <v>173.74</v>
       </c>
       <c r="G984" s="7">
-        <v>19.91</v>
+        <v>43.42</v>
       </c>
       <c r="H984" s="7">
-        <v>34.08</v>
+        <v>75.91</v>
       </c>
     </row>
     <row r="985" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24530,20 +24530,20 @@
         <v>14</v>
       </c>
       <c r="C985" s="8">
-        <v>9214.7999999999993</v>
+        <v>10567.5</v>
       </c>
       <c r="D985" s="6"/>
       <c r="E985" s="7">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="F985" s="7">
-        <v>242.43</v>
+        <v>239.68</v>
       </c>
       <c r="G985" s="7">
-        <v>38.01</v>
+        <v>44.09</v>
       </c>
       <c r="H985" s="7">
-        <v>82</v>
+        <v>103.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   1_satge_volume.xlsx 	modified:   1_stage.xlsx 	modified:   2_stage.xlsx 	modified:   2_stage_volume.xlsx 	modified:   defectura.xlsx 	modified:   expenses.xlsx 	modified:   finish_goods_stocks.xlsx 	renamed:    time_series_11_22.pkl -> forecast/time_series_11_22.pkl 	modified:   raw_mat_bad_stock.xlsx 	modified:   report.pbix 	modified:   sales_extend.xlsx 	modified:   stock_analysis.ipynb 	modified:   stock_analysis.xlsx 	modified:   stock_analysis_final.xlsx 	new file:   time_series_12_22.pkl
</commit_message>
<xml_diff>
--- a/1_stage.xlsx
+++ b/1_stage.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1978" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1982" uniqueCount="148">
   <si>
     <t>Месяц</t>
   </si>
@@ -887,10 +887,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:H986"/>
+  <dimension ref="A1:H988"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A971" workbookViewId="0">
-      <selection activeCell="A981" sqref="A981:H986"/>
+      <selection activeCell="A981" sqref="A981:H988"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="11.45" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24431,23 +24431,23 @@
         <v>147</v>
       </c>
       <c r="B981" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C981" s="8">
-        <v>39782.1</v>
+        <v>1073</v>
       </c>
       <c r="D981" s="6"/>
       <c r="E981" s="7">
-        <v>237.74</v>
+        <v>27.59</v>
       </c>
       <c r="F981" s="7">
-        <v>383.85</v>
+        <v>123.76</v>
       </c>
       <c r="G981" s="7">
-        <v>103.64</v>
+        <v>8.67</v>
       </c>
       <c r="H981" s="7">
-        <v>140.34</v>
+        <v>15.91</v>
       </c>
     </row>
     <row r="982" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24455,23 +24455,23 @@
         <v>147</v>
       </c>
       <c r="B982" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C982" s="8">
-        <v>17997.8</v>
+        <v>69132.5</v>
       </c>
       <c r="D982" s="6"/>
       <c r="E982" s="7">
-        <v>161.25</v>
+        <v>403.75</v>
       </c>
       <c r="F982" s="7">
-        <v>260.57</v>
+        <v>402.99</v>
       </c>
       <c r="G982" s="7">
-        <v>69.069999999999993</v>
+        <v>171.55</v>
       </c>
       <c r="H982" s="7">
-        <v>115.58</v>
+        <v>239.01</v>
       </c>
     </row>
     <row r="983" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24479,23 +24479,23 @@
         <v>147</v>
       </c>
       <c r="B983" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C983" s="5">
-        <v>385.5</v>
+        <v>10</v>
+      </c>
+      <c r="C983" s="8">
+        <v>35691.5</v>
       </c>
       <c r="D983" s="6"/>
       <c r="E983" s="7">
-        <v>18.670000000000002</v>
+        <v>272.92</v>
       </c>
       <c r="F983" s="7">
-        <v>26.28</v>
+        <v>294.85000000000002</v>
       </c>
       <c r="G983" s="7">
-        <v>14.67</v>
+        <v>121.05</v>
       </c>
       <c r="H983" s="7">
-        <v>19.670000000000002</v>
+        <v>201</v>
       </c>
     </row>
     <row r="984" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24503,23 +24503,23 @@
         <v>147</v>
       </c>
       <c r="B984" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C984" s="8">
-        <v>12143.8</v>
+        <v>2444.3000000000002</v>
       </c>
       <c r="D984" s="6"/>
       <c r="E984" s="7">
-        <v>225.75</v>
+        <v>107.75</v>
       </c>
       <c r="F984" s="7">
-        <v>188.51</v>
+        <v>27.8</v>
       </c>
       <c r="G984" s="7">
-        <v>64.42</v>
+        <v>87.91</v>
       </c>
       <c r="H984" s="7">
-        <v>117.91</v>
+        <v>117</v>
       </c>
     </row>
     <row r="985" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24527,23 +24527,23 @@
         <v>147</v>
       </c>
       <c r="B985" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C985" s="8">
-        <v>13704.1</v>
+        <v>4775.5</v>
       </c>
       <c r="D985" s="6"/>
       <c r="E985" s="7">
-        <v>223</v>
+        <v>77.180000000000007</v>
       </c>
       <c r="F985" s="7">
-        <v>234.9</v>
+        <v>250.29</v>
       </c>
       <c r="G985" s="7">
-        <v>58.34</v>
+        <v>19.079999999999998</v>
       </c>
       <c r="H985" s="7">
-        <v>130.5</v>
+        <v>40.57</v>
       </c>
     </row>
     <row r="986" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24551,23 +24551,71 @@
         <v>147</v>
       </c>
       <c r="B986" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C986" s="8">
-        <v>4124</v>
+        <v>21533.7</v>
       </c>
       <c r="D986" s="6"/>
       <c r="E986" s="7">
-        <v>73.010000000000005</v>
+        <v>347.74</v>
       </c>
       <c r="F986" s="7">
-        <v>179.23</v>
+        <v>201.91</v>
       </c>
       <c r="G986" s="7">
-        <v>23.01</v>
+        <v>106.65</v>
       </c>
       <c r="H986" s="7">
-        <v>39.49</v>
+        <v>193.08</v>
+      </c>
+    </row>
+    <row r="987" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A987" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B987" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C987" s="8">
+        <v>30832.9</v>
+      </c>
+      <c r="D987" s="6"/>
+      <c r="E987" s="7">
+        <v>470.66</v>
+      </c>
+      <c r="F987" s="7">
+        <v>228.09</v>
+      </c>
+      <c r="G987" s="7">
+        <v>135.18</v>
+      </c>
+      <c r="H987" s="7">
+        <v>265.83999999999997</v>
+      </c>
+    </row>
+    <row r="988" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A988" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B988" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C988" s="8">
+        <v>5085</v>
+      </c>
+      <c r="D988" s="6"/>
+      <c r="E988" s="7">
+        <v>88.67</v>
+      </c>
+      <c r="F988" s="7">
+        <v>182.65</v>
+      </c>
+      <c r="G988" s="7">
+        <v>27.84</v>
+      </c>
+      <c r="H988" s="7">
+        <v>47.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   1_satge_volume.xlsx 	modified:   1_stage.xlsx 	modified:   2_stage.xlsx 	modified:   2_stage_volume.xlsx 	modified:   defectura.xlsx 	modified:   expenses.xlsx 	modified:   finish_goods_stocks.xlsx 	modified:   raw_mat_bad_stock.xlsx 	modified:   report.pbix 	modified:   sales_extend.xlsx 	modified:   stock_analysis.xlsx 	modified:   time_series_12_22.pkl
</commit_message>
<xml_diff>
--- a/1_stage.xlsx
+++ b/1_stage.xlsx
@@ -24434,20 +24434,20 @@
         <v>8</v>
       </c>
       <c r="C981" s="8">
-        <v>1073</v>
+        <v>1693.8</v>
       </c>
       <c r="D981" s="6"/>
       <c r="E981" s="7">
-        <v>27.59</v>
+        <v>37.590000000000003</v>
       </c>
       <c r="F981" s="7">
-        <v>123.76</v>
+        <v>111.07</v>
       </c>
       <c r="G981" s="7">
-        <v>8.67</v>
+        <v>15.25</v>
       </c>
       <c r="H981" s="7">
-        <v>15.91</v>
+        <v>26.41</v>
       </c>
     </row>
     <row r="982" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24458,20 +24458,20 @@
         <v>9</v>
       </c>
       <c r="C982" s="8">
-        <v>69132.5</v>
+        <v>94687</v>
       </c>
       <c r="D982" s="6"/>
       <c r="E982" s="7">
-        <v>403.75</v>
+        <v>579.59</v>
       </c>
       <c r="F982" s="7">
-        <v>402.99</v>
+        <v>394.59</v>
       </c>
       <c r="G982" s="7">
-        <v>171.55</v>
+        <v>239.96</v>
       </c>
       <c r="H982" s="7">
-        <v>239.01</v>
+        <v>332.83</v>
       </c>
     </row>
     <row r="983" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24482,20 +24482,20 @@
         <v>10</v>
       </c>
       <c r="C983" s="8">
-        <v>35691.5</v>
+        <v>44076.4</v>
       </c>
       <c r="D983" s="6"/>
       <c r="E983" s="7">
-        <v>272.92</v>
+        <v>346.74</v>
       </c>
       <c r="F983" s="7">
-        <v>294.85000000000002</v>
+        <v>291.64999999999998</v>
       </c>
       <c r="G983" s="7">
-        <v>121.05</v>
+        <v>151.13</v>
       </c>
       <c r="H983" s="7">
-        <v>201</v>
+        <v>260.33999999999997</v>
       </c>
     </row>
     <row r="984" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24506,20 +24506,20 @@
         <v>11</v>
       </c>
       <c r="C984" s="8">
-        <v>2444.3000000000002</v>
+        <v>3595</v>
       </c>
       <c r="D984" s="6"/>
       <c r="E984" s="7">
-        <v>107.75</v>
+        <v>165.08</v>
       </c>
       <c r="F984" s="7">
-        <v>27.8</v>
+        <v>27.2</v>
       </c>
       <c r="G984" s="7">
-        <v>87.91</v>
+        <v>132.16</v>
       </c>
       <c r="H984" s="7">
-        <v>117</v>
+        <v>178.33</v>
       </c>
     </row>
     <row r="985" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24530,20 +24530,20 @@
         <v>12</v>
       </c>
       <c r="C985" s="8">
-        <v>4775.5</v>
+        <v>20077.3</v>
       </c>
       <c r="D985" s="6"/>
       <c r="E985" s="7">
-        <v>77.180000000000007</v>
+        <v>306.18</v>
       </c>
       <c r="F985" s="7">
-        <v>250.29</v>
+        <v>245.08</v>
       </c>
       <c r="G985" s="7">
-        <v>19.079999999999998</v>
+        <v>81.92</v>
       </c>
       <c r="H985" s="7">
-        <v>40.57</v>
+        <v>161.07</v>
       </c>
     </row>
     <row r="986" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24554,20 +24554,20 @@
         <v>13</v>
       </c>
       <c r="C986" s="8">
-        <v>21533.7</v>
+        <v>33166.199999999997</v>
       </c>
       <c r="D986" s="6"/>
       <c r="E986" s="7">
-        <v>347.74</v>
+        <v>506.91</v>
       </c>
       <c r="F986" s="7">
-        <v>201.91</v>
+        <v>210.59</v>
       </c>
       <c r="G986" s="7">
-        <v>106.65</v>
+        <v>157.49</v>
       </c>
       <c r="H986" s="7">
-        <v>193.08</v>
+        <v>286.75</v>
       </c>
     </row>
     <row r="987" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24578,20 +24578,20 @@
         <v>14</v>
       </c>
       <c r="C987" s="8">
-        <v>30832.9</v>
+        <v>43337.1</v>
       </c>
       <c r="D987" s="6"/>
       <c r="E987" s="7">
-        <v>470.66</v>
+        <v>580.83000000000004</v>
       </c>
       <c r="F987" s="7">
-        <v>228.09</v>
+        <v>240.19</v>
       </c>
       <c r="G987" s="7">
-        <v>135.18</v>
+        <v>180.43</v>
       </c>
       <c r="H987" s="7">
-        <v>265.83999999999997</v>
+        <v>326.08999999999997</v>
       </c>
     </row>
     <row r="988" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
modified:   1_satge_volume.xlsx 	modified:   1_stage.xlsx 	modified:   2_stage.xlsx 	modified:   2_stage_volume.xlsx 	modified:   defectura.xlsx 	modified:   expenses.xlsx 	modified:   raw_mat_bad_stock.xlsx 	modified:   report.pbix 	modified:   sales_extend.xlsx 	modified:   stock_analysis.ipynb
</commit_message>
<xml_diff>
--- a/1_stage.xlsx
+++ b/1_stage.xlsx
@@ -24628,21 +24628,21 @@
       <c r="B989" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C989" s="5">
-        <v>743.5</v>
+      <c r="C989" s="8">
+        <v>2712</v>
       </c>
       <c r="D989" s="6"/>
       <c r="E989" s="7">
-        <v>27.17</v>
+        <v>48.76</v>
       </c>
       <c r="F989" s="7">
-        <v>96.94</v>
+        <v>137.87</v>
       </c>
       <c r="G989" s="7">
-        <v>7.67</v>
+        <v>19.670000000000002</v>
       </c>
       <c r="H989" s="7">
-        <v>14.25</v>
+        <v>35.340000000000003</v>
       </c>
     </row>
     <row r="990" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24653,20 +24653,20 @@
         <v>9</v>
       </c>
       <c r="C990" s="8">
-        <v>39520.800000000003</v>
+        <v>46771.1</v>
       </c>
       <c r="D990" s="6"/>
       <c r="E990" s="7">
-        <v>233.84</v>
+        <v>288.51</v>
       </c>
       <c r="F990" s="7">
-        <v>368.29</v>
+        <v>364.06</v>
       </c>
       <c r="G990" s="7">
-        <v>107.31</v>
+        <v>128.47</v>
       </c>
       <c r="H990" s="7">
-        <v>148.83000000000001</v>
+        <v>179</v>
       </c>
     </row>
     <row r="991" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24677,20 +24677,20 @@
         <v>10</v>
       </c>
       <c r="C991" s="8">
-        <v>22540.5</v>
+        <v>29277.599999999999</v>
       </c>
       <c r="D991" s="6"/>
       <c r="E991" s="7">
-        <v>174.07</v>
+        <v>238.74</v>
       </c>
       <c r="F991" s="7">
-        <v>344.66</v>
+        <v>342.51</v>
       </c>
       <c r="G991" s="7">
-        <v>65.400000000000006</v>
+        <v>85.48</v>
       </c>
       <c r="H991" s="7">
-        <v>111.67</v>
+        <v>154.84</v>
       </c>
     </row>
     <row r="992" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24701,20 +24701,20 @@
         <v>11</v>
       </c>
       <c r="C992" s="8">
-        <v>2516.5</v>
+        <v>3385.3</v>
       </c>
       <c r="D992" s="6"/>
       <c r="E992" s="7">
-        <v>128.08000000000001</v>
+        <v>170.25</v>
       </c>
       <c r="F992" s="7">
-        <v>25.72</v>
+        <v>25.79</v>
       </c>
       <c r="G992" s="7">
-        <v>97.83</v>
+        <v>131.25</v>
       </c>
       <c r="H992" s="7">
-        <v>126.75</v>
+        <v>171.74</v>
       </c>
     </row>
     <row r="993" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24725,20 +24725,20 @@
         <v>12</v>
       </c>
       <c r="C993" s="8">
-        <v>19530.3</v>
+        <v>26903.8</v>
       </c>
       <c r="D993" s="6"/>
       <c r="E993" s="7">
-        <v>238.5</v>
+        <v>340.17</v>
       </c>
       <c r="F993" s="7">
-        <v>236.5</v>
+        <v>235.32</v>
       </c>
       <c r="G993" s="7">
-        <v>82.58</v>
+        <v>114.33</v>
       </c>
       <c r="H993" s="7">
-        <v>130.59</v>
+        <v>184.76</v>
       </c>
     </row>
     <row r="994" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24749,20 +24749,20 @@
         <v>13</v>
       </c>
       <c r="C994" s="8">
-        <v>21107.1</v>
+        <v>26680.1</v>
       </c>
       <c r="D994" s="6"/>
       <c r="E994" s="7">
-        <v>321.68</v>
+        <v>408.02</v>
       </c>
       <c r="F994" s="7">
-        <v>181.99</v>
+        <v>191.75</v>
       </c>
       <c r="G994" s="7">
-        <v>115.98</v>
+        <v>139.13999999999999</v>
       </c>
       <c r="H994" s="7">
-        <v>182</v>
+        <v>228.83</v>
       </c>
     </row>
     <row r="995" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24773,20 +24773,20 @@
         <v>14</v>
       </c>
       <c r="C995" s="8">
-        <v>11167.5</v>
+        <v>14223.5</v>
       </c>
       <c r="D995" s="6"/>
       <c r="E995" s="7">
-        <v>181.26</v>
+        <v>222.25</v>
       </c>
       <c r="F995" s="7">
-        <v>200.89</v>
+        <v>208.4</v>
       </c>
       <c r="G995" s="7">
-        <v>55.59</v>
+        <v>68.25</v>
       </c>
       <c r="H995" s="7">
-        <v>103.17</v>
+        <v>125.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   1_satge_volume.xlsx 	modified:   1_stage.xlsx 	modified:   2_stage.xlsx 	modified:   2_stage_volume.xlsx 	modified:   defectura.xlsx 	modified:   expenses.xlsx 	modified:   finish_goods_stocks.xlsx 	renamed:    time_series_12_22.pkl -> forecast/time_series_12_22.pkl 	modified:   raw_mat_bad_stock.xlsx 	modified:   report.pbix 	modified:   sales_extend.xlsx 	modified:   stock_analysis.ipynb 	modified:   stock_analysis.xlsx 	modified:   stock_analysis_final.xlsx 	modified:   streamlit_app.py 	new file:   time_series_01_23.pkl
</commit_message>
<xml_diff>
--- a/1_stage.xlsx
+++ b/1_stage.xlsx
@@ -24629,20 +24629,20 @@
         <v>8</v>
       </c>
       <c r="C989" s="8">
-        <v>2712</v>
+        <v>3714.3</v>
       </c>
       <c r="D989" s="6"/>
       <c r="E989" s="7">
-        <v>48.76</v>
+        <v>61.26</v>
       </c>
       <c r="F989" s="7">
-        <v>137.87</v>
+        <v>133.85</v>
       </c>
       <c r="G989" s="7">
-        <v>19.670000000000002</v>
+        <v>27.75</v>
       </c>
       <c r="H989" s="7">
-        <v>35.340000000000003</v>
+        <v>48.34</v>
       </c>
     </row>
     <row r="990" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24653,20 +24653,20 @@
         <v>9</v>
       </c>
       <c r="C990" s="8">
-        <v>46771.1</v>
+        <v>71964.399999999994</v>
       </c>
       <c r="D990" s="6"/>
       <c r="E990" s="7">
-        <v>288.51</v>
+        <v>424</v>
       </c>
       <c r="F990" s="7">
-        <v>364.06</v>
+        <v>359.91</v>
       </c>
       <c r="G990" s="7">
-        <v>128.47</v>
+        <v>199.95</v>
       </c>
       <c r="H990" s="7">
-        <v>179</v>
+        <v>270.5</v>
       </c>
     </row>
     <row r="991" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24677,20 +24677,20 @@
         <v>10</v>
       </c>
       <c r="C991" s="8">
-        <v>29277.599999999999</v>
+        <v>35378.400000000001</v>
       </c>
       <c r="D991" s="6"/>
       <c r="E991" s="7">
-        <v>238.74</v>
+        <v>298.58</v>
       </c>
       <c r="F991" s="7">
-        <v>342.51</v>
+        <v>333.29</v>
       </c>
       <c r="G991" s="7">
-        <v>85.48</v>
+        <v>106.15</v>
       </c>
       <c r="H991" s="7">
-        <v>154.84</v>
+        <v>197.09</v>
       </c>
     </row>
     <row r="992" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24701,20 +24701,20 @@
         <v>11</v>
       </c>
       <c r="C992" s="8">
-        <v>3385.3</v>
+        <v>4565.2</v>
       </c>
       <c r="D992" s="6"/>
       <c r="E992" s="7">
-        <v>170.25</v>
+        <v>224.42</v>
       </c>
       <c r="F992" s="7">
-        <v>25.79</v>
+        <v>26.26</v>
       </c>
       <c r="G992" s="7">
-        <v>131.25</v>
+        <v>173.84</v>
       </c>
       <c r="H992" s="7">
-        <v>171.74</v>
+        <v>229.91</v>
       </c>
     </row>
     <row r="993" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24725,20 +24725,20 @@
         <v>12</v>
       </c>
       <c r="C993" s="8">
-        <v>26903.8</v>
+        <v>37934.199999999997</v>
       </c>
       <c r="D993" s="6"/>
       <c r="E993" s="7">
-        <v>340.17</v>
+        <v>515.17999999999995</v>
       </c>
       <c r="F993" s="7">
-        <v>235.32</v>
+        <v>229.92</v>
       </c>
       <c r="G993" s="7">
-        <v>114.33</v>
+        <v>164.99</v>
       </c>
       <c r="H993" s="7">
-        <v>184.76</v>
+        <v>279.08</v>
       </c>
     </row>
     <row r="994" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24749,20 +24749,20 @@
         <v>13</v>
       </c>
       <c r="C994" s="8">
-        <v>26680.1</v>
+        <v>32959.4</v>
       </c>
       <c r="D994" s="6"/>
       <c r="E994" s="7">
-        <v>408.02</v>
+        <v>508.19</v>
       </c>
       <c r="F994" s="7">
-        <v>191.75</v>
+        <v>195.33</v>
       </c>
       <c r="G994" s="7">
-        <v>139.13999999999999</v>
+        <v>168.74</v>
       </c>
       <c r="H994" s="7">
-        <v>228.83</v>
+        <v>281.41000000000003</v>
       </c>
     </row>
     <row r="995" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24773,20 +24773,20 @@
         <v>14</v>
       </c>
       <c r="C995" s="8">
-        <v>14223.5</v>
+        <v>29442.5</v>
       </c>
       <c r="D995" s="6"/>
       <c r="E995" s="7">
-        <v>222.25</v>
+        <v>366.5</v>
       </c>
       <c r="F995" s="7">
-        <v>208.4</v>
+        <v>225.82</v>
       </c>
       <c r="G995" s="7">
-        <v>68.25</v>
+        <v>130.38</v>
       </c>
       <c r="H995" s="7">
-        <v>125.67</v>
+        <v>229.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   1_satge_volume.xlsx 	modified:   1_stage.xlsx 	modified:   2_stage.xlsx 	modified:   2_stage_volume.xlsx 	modified:   actual_items.xlsx 	modified:   defectura.xlsx 	modified:   expenses.xlsx 	modified:   finish_goods_stocks.xlsx 	renamed:    time_series_01_23.pkl -> forecast/time_series_01_23.pkl 	modified:   raw_mat_bad_stock.xlsx 	modified:   report.pbix 	modified:   sales_extend.xlsx 	modified:   stock_analysis.ipynb 	modified:   stock_analysis.xlsx 	new file:   time_series_02_23.pkl
</commit_message>
<xml_diff>
--- a/1_stage.xlsx
+++ b/1_stage.xlsx
@@ -24824,20 +24824,20 @@
         <v>9</v>
       </c>
       <c r="C997" s="8">
-        <v>18984.8</v>
+        <v>62290.8</v>
       </c>
       <c r="D997" s="6"/>
       <c r="E997" s="7">
-        <v>133.5</v>
+        <v>405.66</v>
       </c>
       <c r="F997" s="7">
-        <v>340.72</v>
+        <v>341.83</v>
       </c>
       <c r="G997" s="7">
-        <v>55.72</v>
+        <v>182.23</v>
       </c>
       <c r="H997" s="7">
-        <v>79.25</v>
+        <v>268.57</v>
       </c>
     </row>
     <row r="998" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24848,20 +24848,20 @@
         <v>10</v>
       </c>
       <c r="C998" s="8">
-        <v>13675.5</v>
+        <v>24759</v>
       </c>
       <c r="D998" s="6"/>
       <c r="E998" s="7">
-        <v>102.24</v>
+        <v>189.42</v>
       </c>
       <c r="F998" s="7">
-        <v>313.73</v>
+        <v>332.02</v>
       </c>
       <c r="G998" s="7">
-        <v>43.59</v>
+        <v>74.569999999999993</v>
       </c>
       <c r="H998" s="7">
-        <v>75.739999999999995</v>
+        <v>134.58000000000001</v>
       </c>
     </row>
     <row r="999" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24871,21 +24871,21 @@
       <c r="B999" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C999" s="5">
-        <v>541</v>
+      <c r="C999" s="8">
+        <v>2850.7</v>
       </c>
       <c r="D999" s="6"/>
       <c r="E999" s="7">
-        <v>26.66</v>
+        <v>123.57</v>
       </c>
       <c r="F999" s="7">
-        <v>26.19</v>
+        <v>28.11</v>
       </c>
       <c r="G999" s="7">
-        <v>20.66</v>
+        <v>101.41</v>
       </c>
       <c r="H999" s="7">
-        <v>29.83</v>
+        <v>132.99</v>
       </c>
     </row>
     <row r="1000" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24896,20 +24896,20 @@
         <v>12</v>
       </c>
       <c r="C1000" s="8">
-        <v>8453.2999999999993</v>
+        <v>32431.4</v>
       </c>
       <c r="D1000" s="6"/>
       <c r="E1000" s="7">
-        <v>138.5</v>
+        <v>544.85</v>
       </c>
       <c r="F1000" s="7">
-        <v>212.72</v>
+        <v>206.45</v>
       </c>
       <c r="G1000" s="7">
-        <v>39.74</v>
+        <v>157.09</v>
       </c>
       <c r="H1000" s="7">
-        <v>73.25</v>
+        <v>300.92</v>
       </c>
     </row>
     <row r="1001" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24920,20 +24920,20 @@
         <v>13</v>
       </c>
       <c r="C1001" s="8">
-        <v>14299.1</v>
+        <v>40872.9</v>
       </c>
       <c r="D1001" s="6"/>
       <c r="E1001" s="7">
-        <v>228.88</v>
+        <v>589.71</v>
       </c>
       <c r="F1001" s="7">
-        <v>210.81</v>
+        <v>228.01</v>
       </c>
       <c r="G1001" s="7">
-        <v>67.83</v>
+        <v>179.26</v>
       </c>
       <c r="H1001" s="7">
-        <v>126.55</v>
+        <v>329.38</v>
       </c>
     </row>
     <row r="1002" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -24944,20 +24944,20 @@
         <v>14</v>
       </c>
       <c r="C1002" s="8">
-        <v>11843.7</v>
+        <v>35034.699999999997</v>
       </c>
       <c r="D1002" s="6"/>
       <c r="E1002" s="7">
-        <v>191.81</v>
+        <v>476.72</v>
       </c>
       <c r="F1002" s="7">
-        <v>215.34</v>
+        <v>233.18</v>
       </c>
       <c r="G1002" s="7">
-        <v>55</v>
+        <v>150.25</v>
       </c>
       <c r="H1002" s="7">
-        <v>108.11</v>
+        <v>267.86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   1_satge_volume.xlsx 	modified:   1_stage.xlsx 	modified:   2_stage.xlsx 	modified:   2_stage_volume.xlsx 	modified:   cost_price 1 stage.xlsx 	modified:   cost_price.xlsx 	modified:   defectura.xlsx 	modified:   expenses.xlsx 	modified:   finish_goods_stocks.xlsx 	renamed:    time_series_02_23.pkl -> forecast/time_series_02_23.pkl 	modified:   raw_mat_bad_stock.xlsx 	modified:   report.pbix 	modified:   sales_extend.xlsx 	modified:   stock_analysis.ipynb 	modified:   stock_analysis.xlsx 	modified:   stock_analysis_final.xlsx 	modified:   streamlit_app.py 	new file:   time_series_03_23.pkl
</commit_message>
<xml_diff>
--- a/1_stage.xlsx
+++ b/1_stage.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2010" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2024" uniqueCount="151">
   <si>
     <t>Месяц</t>
   </si>
@@ -473,6 +473,9 @@
   <si>
     <t>01.02.2023</t>
   </si>
+  <si>
+    <t>01.03.2023</t>
+  </si>
 </sst>
 </file>
 
@@ -893,10 +896,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:H1002"/>
+  <dimension ref="A1:H1009"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A971" workbookViewId="0">
-      <selection activeCell="A996" sqref="A996:H1002"/>
+      <selection activeCell="A1003" sqref="A1003:H1009"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="11.45" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24960,6 +24963,174 @@
         <v>267.86</v>
       </c>
     </row>
+    <row r="1003" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1003" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1003" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1003" s="8">
+        <v>5821.4</v>
+      </c>
+      <c r="D1003" s="6"/>
+      <c r="E1003" s="7">
+        <v>65.989999999999995</v>
+      </c>
+      <c r="F1003" s="7">
+        <v>137.52000000000001</v>
+      </c>
+      <c r="G1003" s="7">
+        <v>42.33</v>
+      </c>
+      <c r="H1003" s="7">
+        <v>70.33</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1004" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1004" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1004" s="8">
+        <v>65968.800000000003</v>
+      </c>
+      <c r="D1004" s="6"/>
+      <c r="E1004" s="7">
+        <v>513.92999999999995</v>
+      </c>
+      <c r="F1004" s="7">
+        <v>314.95999999999998</v>
+      </c>
+      <c r="G1004" s="7">
+        <v>209.45</v>
+      </c>
+      <c r="H1004" s="7">
+        <v>303.25</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1005" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1005" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1005" s="8">
+        <v>37840.400000000001</v>
+      </c>
+      <c r="D1005" s="6"/>
+      <c r="E1005" s="7">
+        <v>327.99</v>
+      </c>
+      <c r="F1005" s="7">
+        <v>293.38</v>
+      </c>
+      <c r="G1005" s="7">
+        <v>128.97999999999999</v>
+      </c>
+      <c r="H1005" s="7">
+        <v>240.04</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1006" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1006" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1006" s="8">
+        <v>2180.8000000000002</v>
+      </c>
+      <c r="D1006" s="6"/>
+      <c r="E1006" s="7">
+        <v>103.17</v>
+      </c>
+      <c r="F1006" s="7">
+        <v>26.49</v>
+      </c>
+      <c r="G1006" s="7">
+        <v>82.34</v>
+      </c>
+      <c r="H1006" s="7">
+        <v>109.67</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1007" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1007" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1007" s="8">
+        <v>41210.300000000003</v>
+      </c>
+      <c r="D1007" s="6"/>
+      <c r="E1007" s="7">
+        <v>644.69000000000005</v>
+      </c>
+      <c r="F1007" s="7">
+        <v>191.71</v>
+      </c>
+      <c r="G1007" s="7">
+        <v>214.96</v>
+      </c>
+      <c r="H1007" s="7">
+        <v>357.65</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1008" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1008" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1008" s="8">
+        <v>45931.4</v>
+      </c>
+      <c r="D1008" s="6"/>
+      <c r="E1008" s="7">
+        <v>637.33000000000004</v>
+      </c>
+      <c r="F1008" s="7">
+        <v>225.45</v>
+      </c>
+      <c r="G1008" s="7">
+        <v>203.73</v>
+      </c>
+      <c r="H1008" s="7">
+        <v>350.18</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1009" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1009" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1009" s="8">
+        <v>38763.1</v>
+      </c>
+      <c r="D1009" s="6"/>
+      <c r="E1009" s="7">
+        <v>643.84</v>
+      </c>
+      <c r="F1009" s="7">
+        <v>198.71</v>
+      </c>
+      <c r="G1009" s="7">
+        <v>195.07</v>
+      </c>
+      <c r="H1009" s="7">
+        <v>362.66</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H901">
     <sortState ref="A2:H914">

</xml_diff>

<commit_message>
Changes to be committed: 	modified:   1_satge_volume.xlsx 	modified:   1_stage.xlsx 	modified:   2_stage.xlsx 	modified:   2_stage_volume.xlsx 	modified:   cost_price 1 stage.xlsx 	modified:   cost_price.xlsx 	modified:   defectura.xlsx 	modified:   expenses.xlsx 	modified:   raw_mat_bad_stock.xlsx 	modified:   report.pbix 	modified:   sales_extend.xlsx
Changes not staged for commit:
	modified:   finish_goods_stocks.xlsx
</commit_message>
<xml_diff>
--- a/1_stage.xlsx
+++ b/1_stage.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2024" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2038" uniqueCount="152">
   <si>
     <t>Месяц</t>
   </si>
@@ -476,6 +476,9 @@
   <si>
     <t>01.03.2023</t>
   </si>
+  <si>
+    <t>01.04.2023</t>
+  </si>
 </sst>
 </file>
 
@@ -896,10 +899,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:H1009"/>
+  <dimension ref="A1:H1016"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A971" workbookViewId="0">
-      <selection activeCell="A1003" sqref="A1003:H1009"/>
+      <selection activeCell="A1010" sqref="A1010:H1016"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="11.45" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -25131,6 +25134,174 @@
         <v>362.66</v>
       </c>
     </row>
+    <row r="1010" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1010" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1010" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1010" s="8">
+        <v>5011.5</v>
+      </c>
+      <c r="D1010" s="6"/>
+      <c r="E1010" s="7">
+        <v>105.34</v>
+      </c>
+      <c r="F1010" s="7">
+        <v>90.44</v>
+      </c>
+      <c r="G1010" s="7">
+        <v>55.41</v>
+      </c>
+      <c r="H1010" s="7">
+        <v>101.18</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1011" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1011" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1011" s="8">
+        <v>42081.8</v>
+      </c>
+      <c r="D1011" s="6"/>
+      <c r="E1011" s="7">
+        <v>484.92</v>
+      </c>
+      <c r="F1011" s="7">
+        <v>180.28</v>
+      </c>
+      <c r="G1011" s="7">
+        <v>233.42</v>
+      </c>
+      <c r="H1011" s="7">
+        <v>303.67</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1012" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1012" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1012" s="8">
+        <v>31258.6</v>
+      </c>
+      <c r="D1012" s="6"/>
+      <c r="E1012" s="7">
+        <v>203.9</v>
+      </c>
+      <c r="F1012" s="7">
+        <v>243.58</v>
+      </c>
+      <c r="G1012" s="7">
+        <v>128.33000000000001</v>
+      </c>
+      <c r="H1012" s="7">
+        <v>196.41</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1013" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1013" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1013" s="8">
+        <v>1589.1</v>
+      </c>
+      <c r="D1013" s="6"/>
+      <c r="E1013" s="7">
+        <v>72</v>
+      </c>
+      <c r="F1013" s="7">
+        <v>26.74</v>
+      </c>
+      <c r="G1013" s="7">
+        <v>59.42</v>
+      </c>
+      <c r="H1013" s="7">
+        <v>76.5</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1014" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1014" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1014" s="8">
+        <v>28196.7</v>
+      </c>
+      <c r="D1014" s="6"/>
+      <c r="E1014" s="7">
+        <v>403.67</v>
+      </c>
+      <c r="F1014" s="7">
+        <v>235.96</v>
+      </c>
+      <c r="G1014" s="7">
+        <v>119.5</v>
+      </c>
+      <c r="H1014" s="7">
+        <v>216.83</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1015" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1015" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1015" s="8">
+        <v>28697.5</v>
+      </c>
+      <c r="D1015" s="6"/>
+      <c r="E1015" s="7">
+        <v>517.97</v>
+      </c>
+      <c r="F1015" s="7">
+        <v>202.21</v>
+      </c>
+      <c r="G1015" s="7">
+        <v>141.91999999999999</v>
+      </c>
+      <c r="H1015" s="7">
+        <v>281.02</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1016" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1016" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1016" s="8">
+        <v>40997</v>
+      </c>
+      <c r="D1016" s="6"/>
+      <c r="E1016" s="7">
+        <v>503.25</v>
+      </c>
+      <c r="F1016" s="7">
+        <v>220.85</v>
+      </c>
+      <c r="G1016" s="7">
+        <v>185.63</v>
+      </c>
+      <c r="H1016" s="7">
+        <v>312.16000000000003</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H901">
     <sortState ref="A2:H914">

</xml_diff>

<commit_message>
modified:   1_satge_volume.xlsx 	modified:   1_stage.xlsx 	modified:   2_stage.xlsx 	modified:   2_stage_volume.xlsx 	modified:   actual_items.xlsx 	modified:   cost_price 1 stage.xlsx 	modified:   cost_price.xlsx 	modified:   defectura.xlsx 	modified:   expenses.xlsx 	modified:   finish_goods_stocks.xlsx 	renamed:    time_series_03_23.pkl -> forecast/time_series_03_23.pkl 	modified:   raw_mat_bad_stock.xlsx 	modified:   report.pbix 	modified:   sales_extend.xlsx 	modified:   stock_analysis.ipynb 	modified:   stock_analysis.xlsx 	new file:   time_series_04_23.pkl
</commit_message>
<xml_diff>
--- a/1_stage.xlsx
+++ b/1_stage.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2038" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2052" uniqueCount="153">
   <si>
     <t>Месяц</t>
   </si>
@@ -477,6 +477,9 @@
     <t>01.03.2023</t>
   </si>
   <si>
+    <t>01.05.2023</t>
+  </si>
+  <si>
     <t>01.04.2023</t>
   </si>
 </sst>
@@ -899,10 +902,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:H1016"/>
+  <dimension ref="A1:H1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A971" workbookViewId="0">
-      <selection activeCell="A1010" sqref="A1010:H1016"/>
+    <sheetView tabSelected="1" topLeftCell="A995" workbookViewId="0">
+      <selection activeCell="A1017" sqref="A1017:H1023"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="11.45" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -25136,7 +25139,7 @@
     </row>
     <row r="1010" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1010" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B1010" s="4" t="s">
         <v>8</v>
@@ -25160,146 +25163,314 @@
     </row>
     <row r="1011" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1011" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B1011" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C1011" s="8">
-        <v>42081.8</v>
+        <v>52157.8</v>
       </c>
       <c r="D1011" s="6"/>
       <c r="E1011" s="7">
-        <v>484.92</v>
+        <v>484.26</v>
       </c>
       <c r="F1011" s="7">
-        <v>180.28</v>
+        <v>199.33</v>
       </c>
       <c r="G1011" s="7">
-        <v>233.42</v>
+        <v>261.67</v>
       </c>
       <c r="H1011" s="7">
-        <v>303.67</v>
+        <v>348.17</v>
       </c>
     </row>
     <row r="1012" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1012" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B1012" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C1012" s="8">
-        <v>31258.6</v>
+        <v>35970.1</v>
       </c>
       <c r="D1012" s="6"/>
       <c r="E1012" s="7">
-        <v>203.9</v>
+        <v>247.39</v>
       </c>
       <c r="F1012" s="7">
-        <v>243.58</v>
+        <v>244.71</v>
       </c>
       <c r="G1012" s="7">
-        <v>128.33000000000001</v>
+        <v>146.99</v>
       </c>
       <c r="H1012" s="7">
-        <v>196.41</v>
+        <v>235.4</v>
       </c>
     </row>
     <row r="1013" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1013" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B1013" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C1013" s="8">
-        <v>1589.1</v>
+        <v>2238.6999999999998</v>
       </c>
       <c r="D1013" s="6"/>
       <c r="E1013" s="7">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="F1013" s="7">
-        <v>26.74</v>
+        <v>26.21</v>
       </c>
       <c r="G1013" s="7">
-        <v>59.42</v>
+        <v>85.42</v>
       </c>
       <c r="H1013" s="7">
-        <v>76.5</v>
+        <v>113.5</v>
       </c>
     </row>
     <row r="1014" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1014" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B1014" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C1014" s="8">
-        <v>28196.7</v>
+        <v>30395.7</v>
       </c>
       <c r="D1014" s="6"/>
       <c r="E1014" s="7">
-        <v>403.67</v>
+        <v>451.34</v>
       </c>
       <c r="F1014" s="7">
-        <v>235.96</v>
+        <v>229.85</v>
       </c>
       <c r="G1014" s="7">
-        <v>119.5</v>
+        <v>132.24</v>
       </c>
       <c r="H1014" s="7">
-        <v>216.83</v>
+        <v>241.66</v>
       </c>
     </row>
     <row r="1015" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1015" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B1015" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C1015" s="8">
-        <v>28697.5</v>
+        <v>36203</v>
       </c>
       <c r="D1015" s="6"/>
       <c r="E1015" s="7">
-        <v>517.97</v>
+        <v>622.64</v>
       </c>
       <c r="F1015" s="7">
-        <v>202.21</v>
+        <v>206.69</v>
       </c>
       <c r="G1015" s="7">
-        <v>141.91999999999999</v>
+        <v>175.16</v>
       </c>
       <c r="H1015" s="7">
-        <v>281.02</v>
+        <v>336.85</v>
       </c>
     </row>
     <row r="1016" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1016" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B1016" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C1016" s="8">
-        <v>40997</v>
+        <v>44068.4</v>
       </c>
       <c r="D1016" s="6"/>
       <c r="E1016" s="7">
-        <v>503.25</v>
+        <v>606.59</v>
       </c>
       <c r="F1016" s="7">
-        <v>220.85</v>
+        <v>218.4</v>
       </c>
       <c r="G1016" s="7">
-        <v>185.63</v>
+        <v>201.78</v>
       </c>
       <c r="H1016" s="7">
-        <v>312.16000000000003</v>
+        <v>371.16</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1017" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1017" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1017" s="8">
+        <v>13635.3</v>
+      </c>
+      <c r="D1017" s="6"/>
+      <c r="E1017" s="7">
+        <v>180</v>
+      </c>
+      <c r="F1017" s="7">
+        <v>135.93</v>
+      </c>
+      <c r="G1017" s="7">
+        <v>100.31</v>
+      </c>
+      <c r="H1017" s="7">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1018" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1018" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1018" s="8">
+        <v>40428.9</v>
+      </c>
+      <c r="D1018" s="6"/>
+      <c r="E1018" s="7">
+        <v>349.75</v>
+      </c>
+      <c r="F1018" s="7">
+        <v>341</v>
+      </c>
+      <c r="G1018" s="7">
+        <v>118.56</v>
+      </c>
+      <c r="H1018" s="7">
+        <v>191.25</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1019" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1019" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1019" s="5">
+        <v>154</v>
+      </c>
+      <c r="D1019" s="6"/>
+      <c r="E1019" s="7">
+        <v>3</v>
+      </c>
+      <c r="F1019" s="7">
+        <v>229.85</v>
+      </c>
+      <c r="G1019" s="7">
+        <v>0.67</v>
+      </c>
+      <c r="H1019" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1020" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1020" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1020" s="8">
+        <v>1145.2</v>
+      </c>
+      <c r="D1020" s="6"/>
+      <c r="E1020" s="7">
+        <v>55.5</v>
+      </c>
+      <c r="F1020" s="7">
+        <v>25.83</v>
+      </c>
+      <c r="G1020" s="7">
+        <v>44.34</v>
+      </c>
+      <c r="H1020" s="7">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1021" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1021" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1021" s="8">
+        <v>20521</v>
+      </c>
+      <c r="D1021" s="6"/>
+      <c r="E1021" s="7">
+        <v>339.85</v>
+      </c>
+      <c r="F1021" s="7">
+        <v>197.18</v>
+      </c>
+      <c r="G1021" s="7">
+        <v>104.07</v>
+      </c>
+      <c r="H1021" s="7">
+        <v>180.73</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1022" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1022" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1022" s="8">
+        <v>15672.4</v>
+      </c>
+      <c r="D1022" s="6"/>
+      <c r="E1022" s="7">
+        <v>315</v>
+      </c>
+      <c r="F1022" s="7">
+        <v>173.94</v>
+      </c>
+      <c r="G1022" s="7">
+        <v>90.1</v>
+      </c>
+      <c r="H1022" s="7">
+        <v>175.41</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:8" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1023" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1023" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1023" s="8">
+        <v>8290.9</v>
+      </c>
+      <c r="D1023" s="6"/>
+      <c r="E1023" s="7">
+        <v>168.91</v>
+      </c>
+      <c r="F1023" s="7">
+        <v>175.8</v>
+      </c>
+      <c r="G1023" s="7">
+        <v>47.16</v>
+      </c>
+      <c r="H1023" s="7">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>